<commit_message>
Changed the name of Hydro_Pumped --> Hydro_Pumped_EP and Hydro_NonPumped --> Hydro_NonPumped_EP to be consistent with the naming of all other existing plants
</commit_message>
<xml_diff>
--- a/DatabasePrep/GeneratorInfo/generator_info_and_costs.xlsx
+++ b/DatabasePrep/GeneratorInfo/generator_info_and_costs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23913"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11560" yWindow="3340" windowWidth="33560" windowHeight="21340" tabRatio="572" activeTab="3"/>
+    <workbookView xWindow="8860" yWindow="0" windowWidth="33560" windowHeight="21340" tabRatio="572" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="generator_info" sheetId="1" r:id="rId1"/>
@@ -940,14 +940,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>Hydro_NonPumped</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hydro_Pumped</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>Water</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -1157,6 +1149,12 @@
   </si>
   <si>
     <t>storage_energy_capacity_cost_$2007_per_mwh</t>
+  </si>
+  <si>
+    <t>Hydro_NonPumped_EP</t>
+  </si>
+  <si>
+    <t>Hydro_Pumped_EP</t>
   </si>
 </sst>
 </file>
@@ -2482,11 +2480,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2088521320"/>
-        <c:axId val="2088523912"/>
+        <c:axId val="-2070018072"/>
+        <c:axId val="-2070045672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2088521320"/>
+        <c:axId val="-2070018072"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1.0"/>
@@ -2498,12 +2496,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088523912"/>
+        <c:crossAx val="-2070045672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2088523912"/>
+        <c:axId val="-2070045672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2514,13 +2512,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088521320"/>
+        <c:crossAx val="-2070018072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2895,11 +2894,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2088767384"/>
-        <c:axId val="2088764280"/>
+        <c:axId val="-2052863528"/>
+        <c:axId val="-2052866584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2088767384"/>
+        <c:axId val="-2052863528"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1.0"/>
@@ -2911,12 +2910,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088764280"/>
+        <c:crossAx val="-2052866584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2088764280"/>
+        <c:axId val="-2052866584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2927,13 +2926,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088767384"/>
+        <c:crossAx val="-2052863528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3161,11 +3161,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2082247400"/>
-        <c:axId val="2082217240"/>
+        <c:axId val="-2052905608"/>
+        <c:axId val="-2052908696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2082247400"/>
+        <c:axId val="-2052905608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3175,7 +3175,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082217240"/>
+        <c:crossAx val="-2052908696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3183,7 +3183,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2082217240"/>
+        <c:axId val="-2052908696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3194,13 +3194,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082247400"/>
+        <c:crossAx val="-2052905608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3245,6 +3246,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4287,11 +4289,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2090024504"/>
-        <c:axId val="2090027720"/>
+        <c:axId val="-2051533480"/>
+        <c:axId val="-2051530264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2090024504"/>
+        <c:axId val="-2051533480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4301,7 +4303,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090027720"/>
+        <c:crossAx val="-2051530264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4309,7 +4311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2090027720"/>
+        <c:axId val="-2051530264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4320,13 +4322,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090024504"/>
+        <c:crossAx val="-2051533480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5580,11 +5583,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2090088600"/>
-        <c:axId val="2090091640"/>
+        <c:axId val="-2051474968"/>
+        <c:axId val="-2051471896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2090088600"/>
+        <c:axId val="-2051474968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5594,7 +5597,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090091640"/>
+        <c:crossAx val="-2051471896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5602,7 +5605,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2090091640"/>
+        <c:axId val="-2051471896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5613,13 +5616,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090088600"/>
+        <c:crossAx val="-2051474968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6169,10 +6173,10 @@
   <dimension ref="A1:AL109"/>
   <sheetViews>
     <sheetView zoomScale="120" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AK21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AK19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A63"/>
+      <selection pane="bottomRight" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -6202,7 +6206,7 @@
   <sheetData>
     <row r="1" spans="1:38">
       <c r="A1" s="23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>207</v>
@@ -6939,7 +6943,7 @@
         <v>CCGT_EP</v>
       </c>
       <c r="AL6" s="23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:38" s="15" customFormat="1">
@@ -8867,7 +8871,7 @@
         <v>Gas_Steam_Turbine_Cogen_EP</v>
       </c>
       <c r="AL21" s="23" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:38">
@@ -10936,7 +10940,7 @@
         <v>Bio_Solid_Steam_Turbine_Cogen_CCS</v>
       </c>
       <c r="AL37" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:38">
@@ -13659,13 +13663,13 @@
         <v>15</v>
       </c>
       <c r="C60" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D60" s="23">
+        <v>0</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="D60" s="23">
-        <v>0</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="F60" s="23">
         <v>91289</v>
@@ -13759,7 +13763,7 @@
       </c>
       <c r="AK60" s="23" t="str">
         <f t="shared" si="32"/>
-        <v>Hydro_NonPumped</v>
+        <v>Hydro_NonPumped_EP</v>
       </c>
       <c r="AL60" s="23"/>
     </row>
@@ -13771,7 +13775,7 @@
         <v>16</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>211</v>
+        <v>278</v>
       </c>
       <c r="D61" s="23">
         <v>0</v>
@@ -13871,10 +13875,10 @@
       </c>
       <c r="AK61" s="23" t="str">
         <f t="shared" si="32"/>
-        <v>Hydro_Pumped</v>
+        <v>Hydro_Pumped_EP</v>
       </c>
       <c r="AL61" s="23" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:38" s="6" customFormat="1" ht="15" customHeight="1">
@@ -13991,7 +13995,7 @@
         <v>Compressed_Air_Energy_Storage</v>
       </c>
       <c r="AL62" s="22" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:38" s="54" customFormat="1">
@@ -14105,7 +14109,7 @@
         <v>Battery_Storage</v>
       </c>
       <c r="AL63" s="56" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="73" spans="3:14">
@@ -14200,7 +14204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK68"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="125" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -23080,7 +23084,7 @@
       </c>
       <c r="C60" s="23" t="str">
         <f>generator_info!C60</f>
-        <v>Hydro_NonPumped</v>
+        <v>Hydro_NonPumped_EP</v>
       </c>
       <c r="D60" s="23">
         <f>generator_info!D60</f>
@@ -23230,7 +23234,7 @@
       </c>
       <c r="C61" s="23" t="str">
         <f>generator_info!C61</f>
-        <v>Hydro_Pumped</v>
+        <v>Hydro_Pumped_EP</v>
       </c>
       <c r="D61" s="23">
         <f>generator_info!D61</f>
@@ -23825,7 +23829,7 @@
   <dimension ref="A1:L353"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C309" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
@@ -23856,7 +23860,7 @@
     </row>
     <row r="3" spans="1:12" s="23" customFormat="1">
       <c r="B3" s="24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="23" customFormat="1">
@@ -23869,7 +23873,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>155</v>
@@ -23878,7 +23882,7 @@
         <v>77</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E6" s="23" t="s">
         <v>157</v>
@@ -23902,7 +23906,7 @@
         <v>148</v>
       </c>
       <c r="L6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -37159,7 +37163,7 @@
       </c>
       <c r="B333" t="str">
         <f>generator_info!C60</f>
-        <v>Hydro_NonPumped</v>
+        <v>Hydro_NonPumped_EP</v>
       </c>
       <c r="D333" s="23">
         <f t="shared" si="286"/>
@@ -37197,7 +37201,7 @@
       </c>
       <c r="B334" t="str">
         <f>generator_info!C61</f>
-        <v>Hydro_Pumped</v>
+        <v>Hydro_Pumped_EP</v>
       </c>
       <c r="D334" s="23">
         <f t="shared" ref="D334" si="288">D333</f>
@@ -37974,8 +37978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A299" workbookViewId="0">
-      <selection activeCell="C353" sqref="C353"/>
+    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
+      <selection activeCell="D310" sqref="D310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -47801,7 +47805,7 @@
       </c>
       <c r="B328" s="23" t="str">
         <f>generator_costs!B333</f>
-        <v>Hydro_NonPumped</v>
+        <v>Hydro_NonPumped_EP</v>
       </c>
       <c r="C328" s="23">
         <f>generator_costs!C333</f>
@@ -47831,7 +47835,7 @@
       </c>
       <c r="B329" s="23" t="str">
         <f>generator_costs!B334</f>
-        <v>Hydro_Pumped</v>
+        <v>Hydro_Pumped_EP</v>
       </c>
       <c r="C329" s="23">
         <f>generator_costs!C334</f>
@@ -54357,149 +54361,149 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="57" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="58" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="58" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B20" s="59" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="B21" s="59" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="B22" s="59" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="57" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="23" customFormat="1">
       <c r="A26" s="57"/>
       <c r="L26" s="23" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="58" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B27" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L27" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="58" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L28" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="s">
+        <v>233</v>
+      </c>
+      <c r="B30" t="s">
+        <v>234</v>
+      </c>
+      <c r="C30" t="s">
         <v>235</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>236</v>
       </c>
-      <c r="C30" t="s">
-        <v>237</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
+        <v>251</v>
+      </c>
+      <c r="F30" t="s">
+        <v>252</v>
+      </c>
+      <c r="G30" t="s">
+        <v>253</v>
+      </c>
+      <c r="H30" t="s">
+        <v>254</v>
+      </c>
+      <c r="I30" t="s">
         <v>238</v>
       </c>
-      <c r="E30" t="s">
+      <c r="J30" t="s">
+        <v>239</v>
+      </c>
+      <c r="L30" s="59" t="s">
         <v>253</v>
       </c>
-      <c r="F30" t="s">
+      <c r="M30" s="59" t="s">
         <v>254</v>
-      </c>
-      <c r="G30" t="s">
-        <v>255</v>
-      </c>
-      <c r="H30" t="s">
-        <v>256</v>
-      </c>
-      <c r="I30" t="s">
-        <v>240</v>
-      </c>
-      <c r="J30" t="s">
-        <v>241</v>
-      </c>
-      <c r="L30" s="59" t="s">
-        <v>255</v>
-      </c>
-      <c r="M30" s="59" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B31" t="s">
+        <v>241</v>
+      </c>
+      <c r="C31" t="s">
+        <v>242</v>
+      </c>
+      <c r="D31" t="s">
         <v>243</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>244</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F31" t="s">
         <v>245</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
+        <v>247</v>
+      </c>
+      <c r="H31" t="s">
         <v>246</v>
       </c>
-      <c r="F31" t="s">
-        <v>247</v>
-      </c>
-      <c r="G31" t="s">
-        <v>249</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="J31" t="s">
         <v>248</v>
       </c>
-      <c r="J31" t="s">
-        <v>250</v>
-      </c>
       <c r="L31" s="59" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M31" s="59" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -54918,69 +54922,69 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="57" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="58" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="58" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B45" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" t="s">
+        <v>233</v>
+      </c>
+      <c r="B47" t="s">
+        <v>234</v>
+      </c>
+      <c r="C47" t="s">
         <v>235</v>
       </c>
-      <c r="B47" t="s">
+      <c r="D47" t="s">
         <v>236</v>
       </c>
-      <c r="C47" t="s">
+      <c r="E47" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="F47" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="G47" t="s">
         <v>237</v>
-      </c>
-      <c r="D47" t="s">
-        <v>238</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="F47" s="23" t="s">
-        <v>261</v>
-      </c>
-      <c r="G47" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="48" spans="1:13" s="23" customFormat="1">
       <c r="B48" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="D48" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="C48" s="23" t="s">
-        <v>244</v>
-      </c>
-      <c r="D48" s="23" t="s">
-        <v>245</v>
-      </c>
       <c r="E48" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="G48" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="F48" s="23" t="s">
+      <c r="H48" s="23" t="s">
         <v>263</v>
-      </c>
-      <c r="G48" s="23" t="s">
-        <v>264</v>
-      </c>
-      <c r="H48" s="23" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -55043,7 +55047,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -55055,7 +55059,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -55067,7 +55071,7 @@
     <row r="56" spans="1:8" s="23" customFormat="1"/>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -55078,15 +55082,15 @@
     </row>
     <row r="60" spans="1:8">
       <c r="B60" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C60" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B61">
         <f>D49*A58</f>
@@ -55099,7 +55103,7 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B62">
         <f>D50*A58</f>
@@ -55112,12 +55116,12 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B65">
         <f>C61/B49</f>
@@ -55126,7 +55130,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B66" s="23">
         <f>C62/B50</f>
@@ -55135,24 +55139,24 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="59" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B68" s="59"/>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="59" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B69" s="59" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="59" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B70" s="59" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="71" spans="1:2">

</xml_diff>